<commit_message>
Updates: option to disable battery management. Also: estimation of the current gear (does not yet include multple chainrings / slumpf up front
</commit_message>
<xml_diff>
--- a/Documentation/VeloPuter_BillOfMaterials.xlsx
+++ b/Documentation/VeloPuter_BillOfMaterials.xlsx
@@ -29,7 +29,7 @@
     <t>Type nr</t>
   </si>
   <si>
-    <t>Amount </t>
+    <t>Amount</t>
   </si>
   <si>
     <t>URL</t>
@@ -107,13 +107,13 @@
     <t>http://nl.mouser.com/ProductDetail/TE-Connectivity-Neohm/RR03J1R2TB/?qs=sGAEpiMZZMu61qfTUdNhG9gR7%2fu94EVJTNO8aw4Eyuw%3d</t>
   </si>
   <si>
-    <t>1 MOhm </t>
+    <t>1 MOhm</t>
   </si>
   <si>
     <t>http://nl.mouser.com/ProductDetail/Yageo/MFR-25FBF52-1M/?qs=sGAEpiMZZMu61qfTUdNhG0IXHLFuiNndLutPCQjaM9A%3d</t>
   </si>
   <si>
-    <t>3 MOhm </t>
+    <t>3 MOhm</t>
   </si>
   <si>
     <t>http://nl.mouser.com/ProductDetail/Yageo/MFR50SFTE52-3M/?qs=sGAEpiMZZMu61qfTUdNhG0IXHLFuiNnd8Ohx6FKyvoE%3d</t>
@@ -182,7 +182,7 @@
     <t>2 Pins</t>
   </si>
   <si>
-    <t>Kan goedkoper maar stekkerbaar is handig </t>
+    <t>Kan goedkoper maar stekkerbaar is handig</t>
   </si>
   <si>
     <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=39511-1002virtualkey53810000virtualkey538-39511-1002</t>
@@ -273,6 +273,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -294,6 +295,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,10 +374,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -383,8 +385,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5255102040816"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.89795918367347"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.0867346938776"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="126.224489795918"/>
@@ -395,6 +396,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -450,15 +452,12 @@
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="E4" s="2" t="n">
         <v>18.97</v>
       </c>
       <c r="F4" s="2" t="n">
         <f aca="false">D4*E4</f>
-        <v>18.97</v>
+        <v>0</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>11</v>
@@ -477,15 +476,12 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="E5" s="2" t="n">
         <v>16.95</v>
       </c>
       <c r="F5" s="2" t="n">
         <f aca="false">D5*E5</f>
-        <v>16.95</v>
+        <v>0</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>15</v>
@@ -504,15 +500,12 @@
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="E6" s="2" t="n">
         <v>4.38</v>
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">D6*E6</f>
-        <v>21.9</v>
+        <v>0</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>19</v>
@@ -553,14 +546,14 @@
         <v>24</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>0.094</v>
       </c>
       <c r="F8" s="2" t="n">
         <f aca="false">D8*E8</f>
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>25</v>
@@ -601,14 +594,14 @@
         <v>28</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0.095</v>
       </c>
       <c r="F10" s="2" t="n">
         <f aca="false">D10*E10</f>
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>29</v>
@@ -625,14 +618,14 @@
         <v>30</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0.094</v>
       </c>
       <c r="F11" s="2" t="n">
         <f aca="false">D11*E11</f>
-        <v>0.094</v>
+        <v>0</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>31</v>
@@ -649,14 +642,14 @@
         <v>32</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.13</v>
       </c>
       <c r="F12" s="2" t="n">
         <f aca="false">D12*E10</f>
-        <v>0.095</v>
+        <v>0</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>33</v>
@@ -745,14 +738,14 @@
         <v>43</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="F16" s="2" t="n">
         <f aca="false">D16*E16</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>44</v>
@@ -769,14 +762,14 @@
         <v>45</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0.09</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">D17*E17</f>
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>46</v>
@@ -1002,15 +995,12 @@
       <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="E26" s="2" t="n">
         <v>1.91</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">D26*E26</f>
-        <v>3.82</v>
+        <v>0</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>71</v>
@@ -1109,7 +1099,142 @@
       </c>
       <c r="F30" s="2" t="n">
         <f aca="false">SUM(F3:F29)</f>
-        <v>79.029</v>
+        <v>16.345</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D38" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D43" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D44" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D46" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D47" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D50" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D51" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D52" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D53" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D54" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D55" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D56" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D57" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D59" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D60" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D61" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D62" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added brakelight timeout. Stops after configured time and also stopns when the bike stopped
</commit_message>
<xml_diff>
--- a/Documentation/VeloPuter_BillOfMaterials.xlsx
+++ b/Documentation/VeloPuter_BillOfMaterials.xlsx
@@ -5,259 +5,264 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="131" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
-    <t>Billl Of Materials</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Type nr</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>PCB</t>
-  </si>
-  <si>
-    <t>~35 EUR per tien</t>
-  </si>
-  <si>
-    <t>https://www.seeedstudio.com/?gclid=CKn9oMPpzNECFYU-Gwodv90Keg</t>
-  </si>
-  <si>
-    <t>Arduino</t>
-  </si>
-  <si>
-    <t>Micro</t>
-  </si>
-  <si>
-    <t>Kloon is goedkoper</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/Genuino/GBX00053/?qs=sGAEpiMZZMuo%252b9%2fB%2fzhRUttOOh91J9FOx%2fpF4THWS1rr5vrGjM0EwQ%3d%3d</t>
-  </si>
-  <si>
-    <t>Oled Display</t>
-  </si>
-  <si>
-    <t>SH1106</t>
-  </si>
-  <si>
-    <t>Zonder garantie: voor de helft op dx.com</t>
-  </si>
-  <si>
-    <t>https://www.hobbyelectronica.nl/product/128x64-oled-wit-i2c-display-1-3inch/</t>
-  </si>
-  <si>
-    <t>Stroom regelaar</t>
-  </si>
-  <si>
-    <t>LDD-700</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=LDD-700Lvirtualkey63430000virtualkey709-LDD-700L</t>
-  </si>
-  <si>
-    <t>Zoomer</t>
-  </si>
-  <si>
-    <t>SD160709</t>
-  </si>
-  <si>
-    <t>https://nl.mouser.com/Search/ProductDetail.aspx?R=SD160709virtualkey52130000virtualkey810-SD160709</t>
-  </si>
-  <si>
-    <t>Weerstand</t>
-  </si>
-  <si>
-    <t>50 kOhm</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/Vishay-Dale/CCF0756K0GKE36/?qs=sGAEpiMZZMu61qfTUdNhG3EzrPz99APht17thdjdK5s%3d</t>
-  </si>
-  <si>
-    <t>100 kOhm</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/Vishay-Dale/CCF07100KJKE36/?qs=sGAEpiMZZMu61qfTUdNhG3bgRPzbhC1waocNI65L68o%3d</t>
-  </si>
-  <si>
-    <t>1 Ohm</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/TE-Connectivity-Neohm/RR03J1R2TB/?qs=sGAEpiMZZMu61qfTUdNhG9gR7%2fu94EVJTNO8aw4Eyuw%3d</t>
-  </si>
-  <si>
-    <t>1 MOhm</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/Yageo/MFR-25FBF52-1M/?qs=sGAEpiMZZMu61qfTUdNhG0IXHLFuiNndLutPCQjaM9A%3d</t>
-  </si>
-  <si>
-    <t>3 MOhm</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/Yageo/MFR50SFTE52-3M/?qs=sGAEpiMZZMu61qfTUdNhG0IXHLFuiNnd8Ohx6FKyvoE%3d</t>
-  </si>
-  <si>
-    <t>Mosfet</t>
-  </si>
-  <si>
-    <t>B7546</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=IRFB7546PBFvirtualkey51120000virtualkey942-IRFB7546PBF</t>
-  </si>
-  <si>
-    <t>5V regelaar</t>
-  </si>
-  <si>
-    <t>LM2931</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/ON-Semiconductor/LM2931T-50G/?qs=sGAEpiMZZMsGz1a6aV8DcIkKCofngvkxldW90XWpkTU%3d</t>
-  </si>
-  <si>
-    <t>Condensator</t>
-  </si>
-  <si>
-    <t>1mF</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=REA102M1ABK-1012Pvirtualkey21980000virtualkey140-REA102M1ABK1012P</t>
-  </si>
-  <si>
-    <t>200 uF</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=227CKS050Mvirtualkey59850000virtualkey598-227CKS050M</t>
-  </si>
-  <si>
-    <t>100 nF</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=1C10Z5U104M050Bvirtualkey61320000virtualkey75-1C10Z5U104M050B</t>
-  </si>
-  <si>
-    <t>Diode</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=1N4148-Tvirtualkey58300000virtualkey583-1N4148-T</t>
-  </si>
-  <si>
-    <t>Zener diode</t>
-  </si>
-  <si>
-    <t>1N5242BTR</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=1N5242BTRvirtualkey51210000virtualkey512-1N5242BTR</t>
-  </si>
-  <si>
-    <t>Connector 2P</t>
-  </si>
-  <si>
-    <t>2 Pins</t>
-  </si>
-  <si>
-    <t>Kan goedkoper maar stekkerbaar is handig</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=39511-1002virtualkey53810000virtualkey538-39511-1002</t>
-  </si>
-  <si>
-    <t>Plug 2P</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=39510-0002virtualkey53810000virtualkey538-39510-0002</t>
-  </si>
-  <si>
-    <t>Connector 4P</t>
-  </si>
-  <si>
-    <t>4 Pins</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=39511-1004virtualkey53810000virtualkey538-39511-1004</t>
-  </si>
-  <si>
-    <t>Plug 4P</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=39510-0004virtualkey53810000virtualkey538-39510-0004</t>
-  </si>
-  <si>
-    <t>Connector 6P</t>
-  </si>
-  <si>
-    <t>6 Pins</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=39511-1006virtualkey53810000virtualkey538-39511-1006</t>
-  </si>
-  <si>
-    <t>plug 6P</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/Search/ProductDetail.aspx?R=39510-0006virtualkey53810000virtualkey538-39510-0006</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>17pins</t>
-  </si>
-  <si>
-    <t>Veel te duur hier</t>
-  </si>
-  <si>
-    <t>http://nl.mouser.com/ProductDetail/3M-Electronic-Solutions-Division/929870-01-17-RB/?qs=sGAEpiMZZMs%252bGHln7q6pm52Y7K%2fp4upyTES9O93eOsk%3d</t>
-  </si>
-  <si>
-    <t>Header + plug</t>
-  </si>
-  <si>
-    <t>8 Pins</t>
-  </si>
-  <si>
-    <t>Per 10</t>
-  </si>
-  <si>
-    <t>http://www.dx.com/p/7s-26awg-8-pin-li-ion-battery-balance-charger-plug-w-cable-10-pcs-301992#.WH_49IhifAQ</t>
-  </si>
-  <si>
-    <t>http://www.dx.com/p/10-x-11-1v-3s1p-jst-xh-connector-adapter-plugs-for-rc-lipo-battery-balance-charger-10-pcs-245231#.WH_4SohifAQ</t>
-  </si>
-  <si>
-    <t>3 Pins</t>
-  </si>
-  <si>
-    <t>http://www.dx.com/p/10-x-7-4v-2s1p-jst-xh-connector-adapter-plug-rc-lipo-battery-balance-charger-b6-250087#.WH_4nohifAQ</t>
-  </si>
-  <si>
-    <t>Totaal</t>
+    <t xml:space="preserve">Billl Of Materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~35 EUR per tien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.seeedstudio.com/?gclid=CKn9oMPpzNECFYU-Gwodv90Keg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kloon is goedkoper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/Genuino/GBX00053/?qs=sGAEpiMZZMuo%252b9%2fB%2fzhRUttOOh91J9FOx%2fpF4THWS1rr5vrGjM0EwQ%3d%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oled Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH1106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonder garantie: voor de helft op dx.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.hobbyelectronica.nl/product/128x64-oled-wit-i2c-display-1-3inch/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stroom regelaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDD-700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=LDD-700Lvirtualkey63430000virtualkey709-LDD-700L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoomer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD160709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/Search/ProductDetail.aspx?R=SD160709virtualkey52130000virtualkey810-SD160709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weerstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 kOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/Vishay-Dale/CCF0756K0GKE36/?qs=sGAEpiMZZMu61qfTUdNhG3EzrPz99APht17thdjdK5s%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 kOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/Vishay-Dale/CCF07100KJKE36/?qs=sGAEpiMZZMu61qfTUdNhG3bgRPzbhC1waocNI65L68o%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/TE-Connectivity-Neohm/RR03J1R2TB/?qs=sGAEpiMZZMu61qfTUdNhG9gR7%2fu94EVJTNO8aw4Eyuw%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 MOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/Yageo/MFR-25FBF52-1M/?qs=sGAEpiMZZMu61qfTUdNhG0IXHLFuiNndLutPCQjaM9A%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 MOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/Yageo/MFR50SFTE52-3M/?qs=sGAEpiMZZMu61qfTUdNhG0IXHLFuiNnd8Ohx6FKyvoE%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosfet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B7546</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=IRFB7546PBFvirtualkey51120000virtualkey942-IRFB7546PBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V regelaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LM2931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/ON-Semiconductor/LM2931T-50G/?qs=sGAEpiMZZMsGz1a6aV8DcIkKCofngvkxldW90XWpkTU%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condensator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1mF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=REA102M1ABK-1012Pvirtualkey21980000virtualkey140-REA102M1ABK1012P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=227CKS050Mvirtualkey59850000virtualkey598-227CKS050M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=1C10Z5U104M050Bvirtualkey61320000virtualkey75-1C10Z5U104M050B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1N4148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=1N4148-Tvirtualkey58300000virtualkey583-1N4148-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zener diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1N5242BTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=1N5242BTRvirtualkey51210000virtualkey512-1N5242BTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector 2P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kan goedkoper maar stekkerbaar is handig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=39511-1002virtualkey53810000virtualkey538-39511-1002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plug 2P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=39510-0002virtualkey53810000virtualkey538-39510-0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector 4P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=39511-1004virtualkey53810000virtualkey538-39511-1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plug 4P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=39510-0004virtualkey53810000virtualkey538-39510-0004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector 6P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=39511-1006virtualkey53810000virtualkey538-39511-1006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plug 6P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/Search/ProductDetail.aspx?R=39510-0006virtualkey53810000virtualkey538-39510-0006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veel te duur hier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://nl.mouser.com/ProductDetail/3M-Electronic-Solutions-Division/929870-01-17-RB/?qs=sGAEpiMZZMs%252bGHln7q6pm52Y7K%2fp4upyTES9O93eOsk%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header + plug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.dx.com/p/7s-26awg-8-pin-li-ion-battery-balance-charger-plug-w-cable-10-pcs-301992#.WH_49IhifAQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.dx.com/p/10-x-11-1v-3s1p-jst-xh-connector-adapter-plugs-for-rc-lipo-battery-balance-charger-10-pcs-245231#.WH_4SohifAQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.dx.com/p/10-x-7-4v-2s1p-jst-xh-connector-adapter-plug-rc-lipo-battery-balance-charger-b6-250087#.WH_4nohifAQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totaal</t>
   </si>
 </sst>
 </file>
@@ -265,7 +270,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
@@ -376,20 +381,20 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="2.89795918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.0867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="126.224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="126.22"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,14 +575,14 @@
         <v>26</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>0.094</v>
       </c>
       <c r="F9" s="2" t="n">
         <f aca="false">D9*E9</f>
-        <v>0.094</v>
+        <v>0</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>27</v>
@@ -738,14 +743,14 @@
         <v>43</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0.2</v>
       </c>
       <c r="F16" s="2" t="n">
         <f aca="false">D16*E16</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>44</v>
@@ -762,14 +767,14 @@
         <v>45</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0.09</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">D17*E17</f>
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>46</v>
@@ -995,12 +1000,15 @@
       <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E26" s="2" t="n">
         <v>1.91</v>
       </c>
       <c r="F26" s="2" t="n">
         <f aca="false">D26*E26</f>
-        <v>0</v>
+        <v>1.91</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>71</v>
@@ -1099,7 +1107,7 @@
       </c>
       <c r="F30" s="2" t="n">
         <f aca="false">SUM(F3:F29)</f>
-        <v>16.345</v>
+        <v>18.451</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,7 +1251,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>